<commit_message>
Working on Step two of Final Project
</commit_message>
<xml_diff>
--- a/data/raw-data/fule_cooking.xlsx
+++ b/data/raw-data/fule_cooking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/mn27712_uga_edu/Documents/DATA BACKUP/MACBOOK AND IPHONE_/Desktop/MADA2025/Mada_final_Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mn27712\OneDrive - University of Georgia\DATA BACKUP\MACBOOK AND IPHONE_\Desktop\MADA2025\Nasir-Mada-Project\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D035C1C-E220-41D5-91E2-E93B5B400A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1D035C1C-E220-41D5-91E2-E93B5B400A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{79A81CF3-1803-42A8-A115-07CAB38A495F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2119,9 +2119,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC272"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="23.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -25919,7 +25924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -25997,6 +26002,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="882513f6-57f1-402e-9cd4-ecb8f5f6b480" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062AF244E107AB5428D9DC167159A3393" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a9722de616b23fae40a3172095eccd93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="882513f6-57f1-402e-9cd4-ecb8f5f6b480" xmlns:ns4="6cb85892-3e52-4f40-966a-40eea172498b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4c2b081c2517e0dc3dd18ae7ac6f8bf" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -26252,26 +26276,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1FDDB2B-1ABC-4D2A-B8C6-143F8EB47AA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6cb85892-3e52-4f40-966a-40eea172498b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="882513f6-57f1-402e-9cd4-ecb8f5f6b480"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="882513f6-57f1-402e-9cd4-ecb8f5f6b480" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7234C60-4F11-4EAB-8ED6-6E4B79D4A89B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6863C159-10A7-41F0-93C7-9CC292F783CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26289,30 +26320,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7234C60-4F11-4EAB-8ED6-6E4B79D4A89B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1FDDB2B-1ABC-4D2A-B8C6-143F8EB47AA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="882513f6-57f1-402e-9cd4-ecb8f5f6b480"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6cb85892-3e52-4f40-966a-40eea172498b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>